<commit_message>
refactor: implement box size assignment and generate Cafe24 upload file
</commit_message>
<xml_diff>
--- a/docs/specification.xlsx
+++ b/docs/specification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yui00\src\prepare-to-pack\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A68D623-44B9-4C4C-99F9-351D7D6FE7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DED836-826A-4D46-9419-0247BCFFD5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{48CDECB9-D0A6-43CF-B923-4C78336F5D59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{48CDECB9-D0A6-43CF-B923-4C78336F5D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Headers" sheetId="6" r:id="rId1"/>
@@ -521,9 +521,6 @@
     <t>box</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -572,9 +569,6 @@
     <t>Add "연번" column</t>
   </si>
   <si>
-    <t>Add a new column called "연번(Serial Number)" as the leftmost column.</t>
-  </si>
-  <si>
     <t>serial_number</t>
   </si>
   <si>
@@ -609,6 +603,12 @@
   </si>
   <si>
     <t>ProcessMultipleItems</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Add a new column called "연번(Serial Number)"</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1063,7 +1063,7 @@
         <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1247,8 +1247,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,23 +1258,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1282,7 +1282,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -1304,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1312,31 +1312,31 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1344,12 +1344,12 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1438,10 +1438,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" t="s">
         <v>160</v>
-      </c>
-      <c r="B31" t="s">
-        <v>161</v>
       </c>
       <c r="C31" t="s">
         <v>159</v>
@@ -1449,15 +1449,15 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C33" s="3">
         <v>73</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34" s="3">
         <v>194</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C35" s="3">
         <v>41</v>
@@ -1481,15 +1481,15 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C37" s="3">
         <v>104</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C38" s="3">
         <v>170</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" s="3">
         <v>266</v>
@@ -1524,7 +1524,7 @@
     <sheetView topLeftCell="B1" zoomScale="101" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1752,10 +1752,10 @@
         <v>123</v>
       </c>
       <c r="F12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12" t="s">
         <v>170</v>
-      </c>
-      <c r="G12" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1786,10 +1786,10 @@
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F14" t="s">
         <v>28</v>
@@ -1872,7 +1872,7 @@
         <v>52</v>
       </c>
       <c r="I18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
@@ -1883,7 +1883,7 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
         <v>28</v>
@@ -1903,7 +1903,7 @@
         <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E20" t="s">
         <v>28</v>
@@ -1923,7 +1923,7 @@
         <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E21" t="s">
         <v>28</v>
@@ -2518,7 +2518,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>